<commit_message>
Refactored Excel generation, added styles.
Signed-off-by: John Griebel <johnkgriebel@gmail.com>
</commit_message>
<xml_diff>
--- a/outputs/Alex Abrines.xlsx
+++ b/outputs/Alex Abrines.xlsx
@@ -343,7 +343,7 @@
     <t>Postup</t>
   </si>
   <si>
-    <t>THree-Point Attempts</t>
+    <t>Three-Point Attempts</t>
   </si>
   <si>
     <t>Spotup</t>
@@ -393,7 +393,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -401,16 +401,39 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ff8080"/>
+        <bgColor rgb="00ff8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b3d9ff"/>
+        <bgColor rgb="00b3d9ff"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001aff8c"/>
+        <bgColor rgb="001aff8c"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -418,12 +441,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -730,1439 +765,1442 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X5" t="s">
+      <c r="X5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" t="n">
+      <c r="A6" s="3" t="n">
         <v>1055.128333333333</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="3" t="n">
         <v>134</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="3" t="n">
         <v>341</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="3" t="n">
         <v>0.393</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="3" t="n">
         <v>94</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="3" t="n">
         <v>247</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="3" t="n">
         <v>0.381</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="3" t="n">
         <v>0.898</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="3" t="n">
         <v>68</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" s="3" t="n">
         <v>86</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N6" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O6" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="P6" t="n">
+      <c r="P6" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="R6" t="n">
+      <c r="R6" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="S6" t="n">
+      <c r="S6" s="3" t="n">
         <v>114</v>
       </c>
-      <c r="T6" t="n">
+      <c r="T6" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="U6" t="n">
+      <c r="U6" s="3" t="n">
         <v>406</v>
       </c>
-      <c r="V6" t="n">
+      <c r="V6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="W6" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" t="n">
+      <c r="W6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" t="n">
+      <c r="A10" s="3" t="n">
         <v>15.5</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="3" t="n">
         <v>0.393</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="3" t="n">
         <v>1.4</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="3" t="n">
         <v>3.6</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="3" t="n">
         <v>0.381</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" s="3" t="n">
         <v>0.898</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10" s="3" t="n">
         <v>1.3</v>
       </c>
-      <c r="N10" t="n">
+      <c r="N10" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="O10" t="n">
+      <c r="O10" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="P10" t="n">
+      <c r="P10" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="Q10" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="R10" t="n">
+      <c r="R10" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="S10" t="n">
+      <c r="S10" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="T10" t="n">
+      <c r="T10" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="U10" t="n">
+      <c r="U10" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" t="n">
+      <c r="V10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U13" t="s">
+      <c r="U13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V13" t="s">
+      <c r="V13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X13" t="s">
+      <c r="X13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" t="n">
+      <c r="A14" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="3" t="n">
         <v>15.2</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="3" t="n">
         <v>0.393</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="3" t="n">
         <v>4.2</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14" s="3" t="n">
         <v>0.381</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" s="3" t="n">
         <v>0.898</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="L14" t="n">
+      <c r="L14" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" s="3" t="n">
         <v>3.8</v>
       </c>
-      <c r="N14" t="n">
+      <c r="N14" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="O14" t="n">
+      <c r="O14" s="3" t="n">
         <v>1.5</v>
       </c>
-      <c r="P14" t="n">
+      <c r="P14" s="3" t="n">
         <v>1.6</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q14" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="R14" t="n">
+      <c r="R14" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="S14" t="n">
+      <c r="S14" s="3" t="n">
         <v>5.1</v>
       </c>
-      <c r="T14" t="n">
+      <c r="T14" s="3" t="n">
         <v>2.3</v>
       </c>
-      <c r="U14" t="n">
+      <c r="U14" s="3" t="n">
         <v>18.1</v>
       </c>
-      <c r="V14" t="n">
-        <v>0</v>
-      </c>
-      <c r="W14" t="n">
-        <v>0</v>
-      </c>
-      <c r="X14" t="n">
+      <c r="V14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V17" t="s">
+      <c r="V17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W17" t="s">
+      <c r="W17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X17" t="s">
+      <c r="X17" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" t="n">
+      <c r="A18" s="3" t="n">
         <v>1055.128333333333</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="3" t="n">
         <v>4.6</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="3" t="n">
         <v>11.6</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="3" t="n">
         <v>0.393</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="3" t="n">
         <v>3.2</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" s="3" t="n">
         <v>8.4</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" s="3" t="n">
         <v>0.381</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="3" t="n">
         <v>1.5</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J18" s="3" t="n">
         <v>0.898</v>
       </c>
-      <c r="K18" t="n">
+      <c r="K18" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="L18" t="n">
+      <c r="L18" s="3" t="n">
         <v>2.3</v>
       </c>
-      <c r="M18" t="n">
+      <c r="M18" s="3" t="n">
         <v>2.9</v>
       </c>
-      <c r="N18" t="n">
+      <c r="N18" s="3" t="n">
         <v>1.4</v>
       </c>
-      <c r="O18" t="n">
+      <c r="O18" s="3" t="n">
         <v>1.1</v>
       </c>
-      <c r="P18" t="n">
+      <c r="P18" s="3" t="n">
         <v>1.3</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="Q18" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="R18" t="n">
+      <c r="R18" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="S18" t="n">
+      <c r="S18" s="3" t="n">
         <v>3.9</v>
       </c>
-      <c r="T18" t="n">
+      <c r="T18" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="U18" t="n">
+      <c r="U18" s="3" t="n">
         <v>13.9</v>
       </c>
-      <c r="V18" t="n">
-        <v>0</v>
-      </c>
-      <c r="W18" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" t="n">
+      <c r="V18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="S21" t="s">
+      <c r="S21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="T21" t="s">
+      <c r="T21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U21" t="s">
+      <c r="U21" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="T22" t="s">
+      <c r="T22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="U22" t="s">
+      <c r="U22" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="S25" t="s">
+      <c r="S25" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T25" t="s">
+      <c r="T25" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" s="3" t="n">
         <v>0.489</v>
       </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" t="n">
+      <c r="F26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3" t="n">
         <v>0.489</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J26" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="K26" t="n">
+      <c r="K26" s="3" t="n">
         <v>0.522</v>
       </c>
-      <c r="L26" t="n">
+      <c r="L26" s="3" t="n">
         <v>0.478</v>
       </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
+      <c r="M26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" s="3" t="n">
         <v>0.522</v>
       </c>
-      <c r="P26" t="n">
+      <c r="P26" s="3" t="n">
         <v>0.478</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="Q26" s="3" t="n">
         <v>0.5599073256840247</v>
       </c>
-      <c r="R26" t="n">
+      <c r="R26" s="3" t="n">
         <v>0.7243401759530792</v>
       </c>
-      <c r="S26" t="n">
+      <c r="S26" s="3" t="n">
         <v>0.1436950146627566</v>
       </c>
-      <c r="T26" t="n">
+      <c r="T26" s="3" t="n">
         <v>0.425531914893617</v>
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O30" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31" s="3" t="n">
         <v>65</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" s="3" t="n">
         <v>16.497499465942</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" s="3" t="n">
         <v>1.3846199512482</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F31" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G31" t="n">
+      <c r="G31" s="3" t="n">
         <v>56</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31" s="3" t="n">
         <v>51.785714285714</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" s="3" t="n">
         <v>68.75</v>
       </c>
-      <c r="J31" t="n">
+      <c r="J31" s="3" t="n">
         <v>12.307692307692</v>
       </c>
-      <c r="K31" t="n">
+      <c r="K31" s="3" t="n">
         <v>4.6153846153846</v>
       </c>
-      <c r="L31" t="n">
+      <c r="L31" s="3" t="n">
         <v>12.307692307692</v>
       </c>
-      <c r="M31" t="n">
+      <c r="M31" s="3" t="n">
         <v>3.0769230769231</v>
       </c>
-      <c r="N31" t="n">
+      <c r="N31" s="3" t="n">
         <v>53.846153846154</v>
       </c>
-      <c r="O31" t="n">
+      <c r="O31" s="3" t="n">
         <v>92.25352112676056</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="Q31" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" s="3" t="n">
         <v>2.0304598808289</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" s="3" t="n">
         <v>0.625</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F32" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G32" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32" s="3" t="n">
         <v>16.666666666667</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J32" s="3" t="n">
         <v>12.5</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K32" s="3" t="n">
         <v>12.5</v>
       </c>
-      <c r="L32" t="n">
+      <c r="L32" s="3" t="n">
         <v>12.5</v>
       </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
+      <c r="M32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="O32" s="3" t="n"/>
+      <c r="Q32" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:24">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" s="3" t="n">
         <v>6.3451800346375</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" s="3" t="n">
         <v>0.72000002861023</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E33" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F33" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G33" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="H33" t="n">
+      <c r="H33" s="3" t="n">
         <v>42.105263157895</v>
       </c>
-      <c r="I33" t="n">
+      <c r="I33" s="3" t="n">
         <v>44.736842105263</v>
       </c>
-      <c r="J33" t="n">
+      <c r="J33" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K33" t="n">
+      <c r="K33" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="n">
+      <c r="L33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="O33" t="n">
+      <c r="O33" s="3" t="n">
         <v>30.66202090592334</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="Q33" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:24">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" s="3" t="n">
         <v>2.2842600345612</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="3" t="n">
         <v>1.6666699647903</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F34" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H34" s="3" t="n">
         <v>55.555555555556</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I34" s="3" t="n">
         <v>83.333333333333</v>
       </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" t="n">
+      <c r="J34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" s="3" t="n">
         <v>55.555555555556</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="O34" s="3" t="n"/>
+      <c r="Q34" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="Q35" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36" s="3" t="n">
         <v>173</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" s="3" t="n">
         <v>43.908599853516</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" s="3" t="n">
         <v>1.1387300491333</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36" s="3" t="n">
         <v>197</v>
       </c>
-      <c r="F36" t="n">
+      <c r="F36" s="3" t="n">
         <v>66</v>
       </c>
-      <c r="G36" t="n">
+      <c r="G36" s="3" t="n">
         <v>168</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H36" s="3" t="n">
         <v>39.285714285714</v>
       </c>
-      <c r="I36" t="n">
+      <c r="I36" s="3" t="n">
         <v>56.25</v>
       </c>
-      <c r="J36" t="n">
+      <c r="J36" s="3" t="n">
         <v>2.3121387283237</v>
       </c>
-      <c r="K36" t="n">
+      <c r="K36" s="3" t="n">
         <v>0.57803468208092</v>
       </c>
-      <c r="L36" t="n">
+      <c r="L36" s="3" t="n">
         <v>1.7341040462428</v>
       </c>
-      <c r="M36" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" t="n">
+      <c r="M36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" s="3" t="n">
         <v>40.462427745665</v>
       </c>
-      <c r="O36" t="n">
+      <c r="O36" s="3" t="n">
         <v>83.02752293577981</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="Q36" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" s="3" t="n">
         <v>6.5989799499512</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" s="3" t="n">
         <v>0.46153798699379</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="F37" t="n">
+      <c r="F37" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G37" t="n">
+      <c r="G37" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="H37" t="n">
+      <c r="H37" s="3" t="n">
         <v>23.809523809524</v>
       </c>
-      <c r="I37" t="n">
+      <c r="I37" s="3" t="n">
         <v>26.190476190476</v>
       </c>
-      <c r="J37" t="n">
+      <c r="J37" s="3" t="n">
         <v>3.8461538461538</v>
       </c>
-      <c r="K37" t="n">
+      <c r="K37" s="3" t="n">
         <v>19.230769230769</v>
       </c>
-      <c r="L37" t="n">
+      <c r="L37" s="3" t="n">
         <v>3.8461538461538</v>
       </c>
-      <c r="M37" t="n">
+      <c r="M37" s="3" t="n">
         <v>3.8461538461538</v>
       </c>
-      <c r="N37" t="n">
+      <c r="N37" s="3" t="n">
         <v>19.230769230769</v>
       </c>
-      <c r="O37" t="n">
+      <c r="O37" s="3" t="n">
         <v>4.184100418410042</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="Q37" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:24">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" s="3" t="n">
         <v>1.0152299404144</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" s="3" t="n">
         <v>1.5</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F38" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G38" t="n">
+      <c r="G38" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H38" t="n">
+      <c r="H38" s="3" t="n">
         <v>75</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I38" s="3" t="n">
         <v>75</v>
       </c>
-      <c r="J38" t="n">
+      <c r="J38" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" t="n">
+      <c r="K38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="M38" t="n">
+      <c r="M38" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="N38" t="n">
+      <c r="N38" s="3" t="n">
         <v>75</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="O38" s="3" t="n"/>
+      <c r="Q38" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:24">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" s="3" t="n">
         <v>11.928899765015</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39" s="3" t="n">
         <v>0.78723400831223</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="F39" t="n">
+      <c r="F39" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="G39" t="n">
+      <c r="G39" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="H39" t="n">
+      <c r="H39" s="3" t="n">
         <v>31.707317073171</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39" s="3" t="n">
         <v>40.243902439024</v>
       </c>
-      <c r="J39" t="n">
+      <c r="J39" s="3" t="n">
         <v>4.2553191489362</v>
       </c>
-      <c r="K39" t="n">
+      <c r="K39" s="3" t="n">
         <v>8.510638297872299</v>
       </c>
-      <c r="L39" t="n">
+      <c r="L39" s="3" t="n">
         <v>4.2553191489362</v>
       </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="n">
+      <c r="M39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3" t="n">
         <v>31.914893617021</v>
       </c>
-      <c r="O39" t="n">
+      <c r="O39" s="3" t="n">
         <v>28.85375494071146</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="Q39" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" s="3" t="n">
         <v>2.5380699634552</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="F40" t="n">
+      <c r="F40" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G40" t="n">
+      <c r="G40" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H40" t="n">
+      <c r="H40" s="3" t="n">
         <v>22.222222222222</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I40" s="3" t="n">
         <v>27.777777777778</v>
       </c>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" t="n">
+      <c r="J40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="L40" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" t="n">
+      <c r="L40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O40" t="n">
+      <c r="O40" s="3" t="n">
         <v>1.730103806228374</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="Q40" s="5" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" s="3" t="n">
         <v>6.8527898788452</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41" s="3" t="n">
         <v>0.62963002920151</v>
       </c>
-      <c r="E41" t="n">
+      <c r="E41" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="F41" t="n">
+      <c r="F41" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G41" t="n">
+      <c r="G41" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H41" t="n">
+      <c r="H41" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I41" t="n">
+      <c r="I41" s="3" t="n">
         <v>37.5</v>
       </c>
-      <c r="J41" t="n">
+      <c r="J41" s="3" t="n">
         <v>22.222222222222</v>
       </c>
-      <c r="K41" t="n">
+      <c r="K41" s="3" t="n">
         <v>48.148148148148</v>
       </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" t="n">
+      <c r="L41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3" t="n">
         <v>29.62962962963</v>
       </c>
-      <c r="O41" t="n">
+      <c r="O41" s="3" t="n">
         <v>71.69811320754717</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="Q41" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="Q42" t="s">
+      <c r="Q42" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:24">
-      <c r="Q43" t="s">
+      <c r="Q43" s="5" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>